<commit_message>
Conversions work, formatting tidied up a bit
</commit_message>
<xml_diff>
--- a/conversions.xlsx
+++ b/conversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ferrier\Documents\GitHub\FitnotesLiftoffImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA30D55-F8B7-4D37-A3C2-D2306500C745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C00F689-FB76-463D-B8B0-166BDC52B054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Bicep Curl (Barbell)</t>
   </si>
@@ -216,9 +216,6 @@
     <t>Cable Overhead Triceps Extension</t>
   </si>
   <si>
-    <t>Technogym Seated Machine Fly</t>
-  </si>
-  <si>
     <t>T-Bar Row</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
     <t>shoulder press machine</t>
   </si>
   <si>
-    <t>technogym rear delt</t>
-  </si>
-  <si>
     <t>james grip lat pulldown</t>
   </si>
   <si>
@@ -319,12 +313,6 @@
   </si>
   <si>
     <t>Unmarked</t>
-  </si>
-  <si>
-    <t>Variations</t>
-  </si>
-  <si>
-    <t>vbar ashlyns,V-bar gym group</t>
   </si>
 </sst>
 </file>
@@ -645,7 +633,7 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,27 +648,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
-        <v>98</v>
-      </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,7 +676,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,18 +687,18 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -724,34 +709,34 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -759,7 +744,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -767,7 +752,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -807,13 +792,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -821,15 +806,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -837,39 +822,39 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -877,7 +862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -885,15 +870,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -901,42 +886,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
       </c>
-      <c r="C30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -944,23 +926,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -968,34 +950,31 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>44</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="C37" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -1003,42 +982,39 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>55</v>
       </c>
       <c r="B43" t="s">
         <v>41</v>
       </c>
-      <c r="C43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>57</v>
       </c>

</xml_diff>